<commit_message>
More error pages, bugfixes, code cleanup
</commit_message>
<xml_diff>
--- a/Documentation/Gantt Chart.xlsx
+++ b/Documentation/Gantt Chart.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\David\Documents\Work\University\Year 4\Honours\Honours-Project\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{27AA2615-98C5-4BEF-AC20-DDEA6266AC13}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$11</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$2:$B$11</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$2:$C$15</definedName>
-  </definedNames>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -76,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -131,9 +126,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -250,7 +245,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0E57-4121-A1F5-0E86B201E81A}"/>
             </c:ext>
@@ -357,7 +352,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0E57-4121-A1F5-0E86B201E81A}"/>
             </c:ext>
@@ -491,14 +486,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -529,9 +524,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -644,6 +639,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BF49-4179-BA3A-DF2F41A83A6E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -742,6 +742,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BF49-4179-BA3A-DF2F41A83A6E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -763,6 +768,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -811,11 +817,6 @@
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1368,7 +1369,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="103" workbookViewId="0" zoomToFit="1"/>
@@ -1388,7 +1389,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D747E26A-1FA5-4175-9375-DF55B4D883B0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D747E26A-1FA5-4175-9375-DF55B4D883B0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1428,7 +1429,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1447,12 +1454,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C11" totalsRowShown="0">
-  <autoFilter ref="A1:C11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C11" totalsRowShown="0">
+  <autoFilter ref="A1:C11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="TASK "/>
-    <tableColumn id="2" name="Start date " dataDxfId="0"/>
-    <tableColumn id="3" name="Days to complete "/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TASK "/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Start date " dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Days to complete "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1747,18 +1754,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>